<commit_message>
feat: add tileset slicer and tileset-backed neon map
</commit_message>
<xml_diff>
--- a/example/game_05_neon_aberration/map_tiles.xlsx
+++ b/example/game_05_neon_aberration/map_tiles.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A4:I9"/>
+  <dimension ref="A4:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -430,6 +430,21 @@
       <c r="I4" t="str">
         <v>string</v>
       </c>
+      <c r="J4" t="str">
+        <v>string</v>
+      </c>
+      <c r="K4" t="str">
+        <v>uint</v>
+      </c>
+      <c r="L4" t="str">
+        <v>uint</v>
+      </c>
+      <c r="M4" t="str">
+        <v>uint</v>
+      </c>
+      <c r="N4" t="str">
+        <v>uint</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -459,6 +474,21 @@
       <c r="I5" t="str">
         <v>connections</v>
       </c>
+      <c r="J5" t="str">
+        <v>tileSheet</v>
+      </c>
+      <c r="K5" t="str">
+        <v>tileWidth</v>
+      </c>
+      <c r="L5" t="str">
+        <v>tileHeight</v>
+      </c>
+      <c r="M5" t="str">
+        <v>tileRow</v>
+      </c>
+      <c r="N5" t="str">
+        <v>tileCol</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -488,6 +518,21 @@
       <c r="I6" t="str">
         <v>District-Helix|District-Nadir</v>
       </c>
+      <c r="J6" t="str">
+        <v>tileset_city</v>
+      </c>
+      <c r="K6" t="str">
+        <v>32</v>
+      </c>
+      <c r="L6" t="str">
+        <v>32</v>
+      </c>
+      <c r="M6" t="str">
+        <v>0</v>
+      </c>
+      <c r="N6" t="str">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -517,6 +562,21 @@
       <c r="I7" t="str">
         <v>District-Helix|Harbor Nexus</v>
       </c>
+      <c r="J7" t="str">
+        <v>tileset_city</v>
+      </c>
+      <c r="K7" t="str">
+        <v>32</v>
+      </c>
+      <c r="L7" t="str">
+        <v>32</v>
+      </c>
+      <c r="M7" t="str">
+        <v>0</v>
+      </c>
+      <c r="N7" t="str">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -546,6 +606,21 @@
       <c r="I8" t="str">
         <v>Harbor Nexus|Rift-13</v>
       </c>
+      <c r="J8" t="str">
+        <v>tileset_city</v>
+      </c>
+      <c r="K8" t="str">
+        <v>32</v>
+      </c>
+      <c r="L8" t="str">
+        <v>32</v>
+      </c>
+      <c r="M8" t="str">
+        <v>1</v>
+      </c>
+      <c r="N8" t="str">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -575,10 +650,25 @@
       <c r="I9" t="str">
         <v>Rift-13</v>
       </c>
+      <c r="J9" t="str">
+        <v>tileset_city</v>
+      </c>
+      <c r="K9" t="str">
+        <v>32</v>
+      </c>
+      <c r="L9" t="str">
+        <v>32</v>
+      </c>
+      <c r="M9" t="str">
+        <v>1</v>
+      </c>
+      <c r="N9" t="str">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A4:I9"/>
+    <ignoredError numberStoredAsText="1" sqref="A4:N9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>